<commit_message>
some restructuring, getting time matrix works now, has been built on a docker image and can be started from there
</commit_message>
<xml_diff>
--- a/Kund1/september_clean/September_arbete.xlsx
+++ b/Kund1/september_clean/September_arbete.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eriksimertnordgren/Desktop/OptimalRoutePlanning/code/Kund1/september_clean/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eriksimertnordgren/Desktop/OptimalRoutePlanning/code/tsp_multiple_days/Kund1/september_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC21B32-59C2-B746-BF2A-9E37F58E3DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EAE815-B702-544D-809D-51A6B43BBBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25354" uniqueCount="1277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25360" uniqueCount="1277">
   <si>
     <t>Dag</t>
   </si>
@@ -4391,8 +4391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
+      <selection activeCell="H327" sqref="H327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6960,6 +6960,9 @@
       <c r="F38" t="s">
         <v>32</v>
       </c>
+      <c r="G38" t="s">
+        <v>396</v>
+      </c>
       <c r="I38">
         <v>4805</v>
       </c>
@@ -7025,6 +7028,9 @@
       <c r="F39" t="s">
         <v>32</v>
       </c>
+      <c r="G39" t="s">
+        <v>396</v>
+      </c>
       <c r="I39">
         <v>4805</v>
       </c>
@@ -17504,6 +17510,9 @@
       <c r="F195" t="s">
         <v>32</v>
       </c>
+      <c r="G195" t="s">
+        <v>396</v>
+      </c>
       <c r="I195">
         <v>4805</v>
       </c>
@@ -17569,6 +17578,9 @@
       <c r="F196" t="s">
         <v>32</v>
       </c>
+      <c r="G196" t="s">
+        <v>396</v>
+      </c>
       <c r="I196">
         <v>4805</v>
       </c>
@@ -26032,6 +26044,9 @@
       <c r="F322" t="s">
         <v>32</v>
       </c>
+      <c r="G322" t="s">
+        <v>396</v>
+      </c>
       <c r="I322">
         <v>4805</v>
       </c>
@@ -26099,6 +26114,9 @@
       </c>
       <c r="F323" t="s">
         <v>32</v>
+      </c>
+      <c r="G323" t="s">
+        <v>396</v>
       </c>
       <c r="I323">
         <v>4805</v>

</xml_diff>